<commit_message>
Run the 2nd Notebook to deliver
</commit_message>
<xml_diff>
--- a/[ML]_Project_EDAOutputs_Group33/FeatureSelection/Feature_Selection_Results_LogisticRegression_ScaledData.xlsx
+++ b/[ML]_Project_EDAOutputs_Group33/FeatureSelection/Feature_Selection_Results_LogisticRegression_ScaledData.xlsx
@@ -828,17 +828,25 @@
           <t>COVID-19 Indicator</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>lasso</t>
+        </is>
+      </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>lasso</t>
+        </is>
+      </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">

</xml_diff>